<commit_message>
updated notebook with GAP assays
</commit_message>
<xml_diff>
--- a/mathy/labnotebook/dn_mutant_expression.xlsx
+++ b/mathy/labnotebook/dn_mutant_expression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjmathy/gdrive/gsp1_dms/mathy/labnotebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FA29AD-4DC0-594F-BB78-E47ABEA3D3B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13FE7FF-428B-DF4C-BD08-7054D5FB9F90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33720" yWindow="-680" windowWidth="28800" windowHeight="17540" xr2:uid="{FDBDDF14-62F9-D34E-B8B1-40166B37920C}"/>
+    <workbookView xWindow="-36040" yWindow="800" windowWidth="28800" windowHeight="17540" xr2:uid="{FDBDDF14-62F9-D34E-B8B1-40166B37920C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>construct label</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>5x40 uL, 1.6 mM</t>
+  </si>
+  <si>
+    <t>9x30 uL, 2 mM</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -720,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD36135B-5CE3-FB46-9380-725FC4468D58}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +743,7 @@
     <col min="8" max="8" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +775,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>68</v>
       </c>
@@ -783,13 +789,15 @@
       <c r="E2" s="7"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="H2" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="I2" s="15"/>
       <c r="J2" s="17">
         <v>37675</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -813,7 +821,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -837,7 +845,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -861,7 +869,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -884,8 +892,11 @@
       <c r="J6" s="17">
         <v>37675</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -909,7 +920,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -933,7 +944,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -957,7 +968,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -981,7 +992,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +1016,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1040,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1064,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -1077,7 +1088,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1101,7 +1112,7 @@
         <v>37675</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>

</xml_diff>